<commit_message>
Added placeholder statement for ddck files.
</commit_message>
<xml_diff>
--- a/dev-tools/componentOverview.xlsx
+++ b/dev-tools/componentOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\pytrnsys\dev-tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2.2\Internship\pytrnsys\dev-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A234A-CC28-4090-8AF6-BEEF5AE91F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1CB9E-3FBA-485F-B2AB-167C8CE703DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t>folder</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>weather</t>
+  </si>
+  <si>
+    <t>const_eff_hx, const_eff_hx_dhw, const_eff_hx_dhw_contr, const_eff_hx_dhw_pid, const_eff_hx_regeneration, const_eff_hx_solarIce, const_eff_hx_solarIceSlurry</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Automatic Connection Feature Completed</t>
   </si>
 </sst>
 </file>
@@ -243,15 +252,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -259,14 +280,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30BD51A-C333-4CFC-8B6A-72B296EA6787}">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,391 +641,471 @@
     <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="D6" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="D8" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="D9" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D11" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D20" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D21" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="D22" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D23" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D24" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D25" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="B26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="D27" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="D28" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="B30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D31" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="C33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+      <c r="D34" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="D35" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
+      <c r="B36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added placeholder statements in Water Tap
</commit_message>
<xml_diff>
--- a/dev-tools/componentOverview.xlsx
+++ b/dev-tools/componentOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2.2\Internship\pytrnsys\dev-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA1CB9E-3FBA-485F-B2AB-167C8CE703DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE8D68-857C-47DC-B1DE-FB86F4796EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>folder</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>Automatic Connection Feature Completed</t>
+  </si>
+  <si>
+    <t>demands\dhw</t>
+  </si>
+  <si>
+    <t>WTap</t>
+  </si>
+  <si>
+    <t>dhw_mfh,  dhw_mfh_1hour, dhw_mfh_CCT, dhw_mfh_v1, dhw_sfh_task44</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,16 +642,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30BD51A-C333-4CFC-8B6A-72B296EA6787}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1104,6 +1116,20 @@
       </c>
       <c r="D36" s="3"/>
     </row>
+    <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Add placeholder statements to ddck
</commit_message>
<xml_diff>
--- a/dev-tools/componentOverview.xlsx
+++ b/dev-tools/componentOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2.2\Internship\pytrnsys\dev-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE8D68-857C-47DC-B1DE-FB86F4796EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5222512A-F2B5-4ECF-8A6A-3FE3F5F50CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>folder</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Automatic Connection Feature Completed</t>
-  </si>
-  <si>
     <t>demands\dhw</t>
   </si>
   <si>
@@ -238,6 +235,12 @@
   </si>
   <si>
     <t>dhw_mfh,  dhw_mfh_1hour, dhw_mfh_CCT, dhw_mfh_v1, dhw_sfh_task44</t>
+  </si>
+  <si>
+    <t>Automatic Connection Feature Completed, Updated port names</t>
+  </si>
+  <si>
+    <t>Automatic Connection Feature Completed (Both inputs and outputs)</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,7 +656,7 @@
     <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -693,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -705,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -731,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -757,7 +760,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -769,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,7 +798,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -893,7 +896,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -907,7 +910,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -921,7 +924,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -935,7 +938,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,7 +950,7 @@
         <v>38</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,7 +964,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -975,7 +978,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,7 +1004,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1013,7 +1016,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1051,7 +1054,7 @@
         <v>54</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1089,7 +1092,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1101,7 +1104,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,16 +1121,16 @@
     </row>
     <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge pull request #121 from SPF-OST/output-placeholders"
</commit_message>
<xml_diff>
--- a/dev-tools/componentOverview.xlsx
+++ b/dev-tools/componentOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2.2\Internship\pytrnsys\dev-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5222512A-F2B5-4ECF-8A6A-3FE3F5F50CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE8D68-857C-47DC-B1DE-FB86F4796EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
   <si>
     <t>folder</t>
   </si>
@@ -228,6 +228,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Automatic Connection Feature Completed</t>
+  </si>
+  <si>
     <t>demands\dhw</t>
   </si>
   <si>
@@ -235,12 +238,6 @@
   </si>
   <si>
     <t>dhw_mfh,  dhw_mfh_1hour, dhw_mfh_CCT, dhw_mfh_v1, dhw_sfh_task44</t>
-  </si>
-  <si>
-    <t>Automatic Connection Feature Completed, Updated port names</t>
-  </si>
-  <si>
-    <t>Automatic Connection Feature Completed (Both inputs and outputs)</t>
   </si>
 </sst>
 </file>
@@ -648,7 +645,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +653,7 @@
     <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -696,7 +693,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -708,7 +705,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -734,7 +731,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -760,7 +757,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -772,7 +769,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -798,7 +795,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -896,7 +893,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -910,7 +907,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -924,7 +921,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -938,7 +935,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -950,7 +947,7 @@
         <v>38</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -964,7 +961,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -978,7 +975,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1004,7 +1001,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1016,7 +1013,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1054,7 +1051,7 @@
         <v>54</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1092,7 +1089,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1104,7 +1101,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1121,16 +1118,16 @@
     </row>
     <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="D37" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge pull request #121 from SPF-OST/output-placeholders""
</commit_message>
<xml_diff>
--- a/dev-tools/componentOverview.xlsx
+++ b/dev-tools/componentOverview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\2.2\Internship\pytrnsys\dev-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE8D68-857C-47DC-B1DE-FB86F4796EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5222512A-F2B5-4ECF-8A6A-3FE3F5F50CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0B68507-0D55-4F8F-B617-669BA83A2A84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>folder</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Automatic Connection Feature Completed</t>
-  </si>
-  <si>
     <t>demands\dhw</t>
   </si>
   <si>
@@ -238,6 +235,12 @@
   </si>
   <si>
     <t>dhw_mfh,  dhw_mfh_1hour, dhw_mfh_CCT, dhw_mfh_v1, dhw_sfh_task44</t>
+  </si>
+  <si>
+    <t>Automatic Connection Feature Completed, Updated port names</t>
+  </si>
+  <si>
+    <t>Automatic Connection Feature Completed (Both inputs and outputs)</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,7 +656,7 @@
     <col min="1" max="1" width="54.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -693,7 +696,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -705,7 +708,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -731,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -757,7 +760,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -769,7 +772,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -795,7 +798,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -893,7 +896,7 @@
         <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="97.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -907,7 +910,7 @@
         <v>33</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -921,7 +924,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -935,7 +938,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,7 +950,7 @@
         <v>38</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,7 +964,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -975,7 +978,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1001,7 +1004,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1013,7 +1016,7 @@
         <v>49</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1051,7 +1054,7 @@
         <v>54</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1089,7 +1092,7 @@
         <v>54</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1101,7 +1104,7 @@
         <v>54</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,16 +1121,16 @@
     </row>
     <row r="37" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>